<commit_message>
6.0 - base route
</commit_message>
<xml_diff>
--- a/09-golfklub/vegpontok.xlsx
+++ b/09-golfklub/vegpontok.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://szaszbp-my.sharepoint.com/personal/boros_sandor_logiker_hu/Documents/2024/Express_gyakorlatok/09-golfklub/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="11_AD4D6204247ACDAA4110B405E1D1D9C4693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE55C11F-379B-49EA-9978-72CA9A83E71D}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="11_AD4D6204247ACDAA4110B405E1D1D9C4693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45A3B2DA-DE39-4838-B803-BDCE258DE214}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="95">
   <si>
     <t>végpont</t>
   </si>
@@ -57,9 +57,6 @@
     <t>befizetesekadattabla</t>
   </si>
   <si>
-    <t>SELECT * FROM</t>
-  </si>
-  <si>
     <t>get</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
   </si>
   <si>
     <t>patch</t>
-  </si>
-  <si>
-    <t>helyimenütartozikhozzá</t>
   </si>
   <si>
     <t>adatbazis muvelet</t>
@@ -244,21 +238,9 @@
     <t>http://localhost:3000/golf/login</t>
   </si>
   <si>
-    <t>http://localhost:3000/golf/befizetesek/:uazon</t>
-  </si>
-  <si>
     <t>http://localhost:3000/golf/befizetes</t>
   </si>
   <si>
-    <t>http://localhost:3000/golf/ugyfelek/:uazon</t>
-  </si>
-  <si>
-    <t>http://localhost:3000/golf/tagsagok</t>
-  </si>
-  <si>
-    <t>http://localhost:3000/golf/tagsagok/:uazon</t>
-  </si>
-  <si>
     <t>http://localhost:3000/golf/jelenlet</t>
   </si>
   <si>
@@ -299,13 +281,67 @@
   </si>
   <si>
     <t>befizetes</t>
+  </si>
+  <si>
+    <t>tagdíj befizetése</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/golf/befizetes/:uazon</t>
+  </si>
+  <si>
+    <t>összes ügyfél befizetésének a listája</t>
+  </si>
+  <si>
+    <t>adott ügyfél befizetéseinek a lekérdezése</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/golf/ugyfelek</t>
+  </si>
+  <si>
+    <t>tagdíj befizetés módosítása (csak összeg)</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/golf/befizetes/:uazon/:bido</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/golf/tagsag/:uazon</t>
+  </si>
+  <si>
+    <t>adott tag tagságainak a változása</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/golf/tagsag/:uazon/:tszint</t>
+  </si>
+  <si>
+    <t>minden látogatás</t>
+  </si>
+  <si>
+    <t>adott ügyfél látogatásai</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/golf/jelenlet/:uazon</t>
+  </si>
+  <si>
+    <t>adott ügyfél belép</t>
+  </si>
+  <si>
+    <t>adott ügyfél kilép</t>
+  </si>
+  <si>
+    <t>tagsági szint módosítása</t>
+  </si>
+  <si>
+    <t>tagsag</t>
+  </si>
+  <si>
+    <t>jelenlet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,13 +359,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="24"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -417,7 +446,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -438,11 +467,23 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -774,7 +815,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="A1:F9"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -789,22 +830,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
-      </c>
-      <c r="E1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -812,16 +853,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>28</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" t="s">
-        <v>30</v>
       </c>
       <c r="F2" s="7">
         <v>31121</v>
@@ -832,16 +873,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
         <v>31</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>32</v>
-      </c>
-      <c r="D3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" t="s">
-        <v>34</v>
       </c>
       <c r="F3" s="7">
         <v>33048</v>
@@ -852,16 +893,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
         <v>35</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>36</v>
-      </c>
-      <c r="D4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" t="s">
-        <v>38</v>
       </c>
       <c r="F4" s="7">
         <v>28829</v>
@@ -872,16 +913,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
         <v>39</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>40</v>
-      </c>
-      <c r="D5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" t="s">
-        <v>42</v>
       </c>
       <c r="F5" s="7">
         <v>32346</v>
@@ -892,16 +933,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
         <v>43</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>44</v>
-      </c>
-      <c r="D6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" t="s">
-        <v>46</v>
       </c>
       <c r="F6" s="7">
         <v>29352</v>
@@ -912,16 +953,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
         <v>47</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>48</v>
-      </c>
-      <c r="D7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" t="s">
-        <v>50</v>
       </c>
       <c r="F7" s="7">
         <v>34951</v>
@@ -932,16 +973,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
         <v>51</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>52</v>
-      </c>
-      <c r="D8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" t="s">
-        <v>54</v>
       </c>
       <c r="F8" s="7">
         <v>30000</v>
@@ -952,16 +993,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" t="s">
         <v>55</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>56</v>
-      </c>
-      <c r="D9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" t="s">
-        <v>58</v>
       </c>
       <c r="F9" s="7">
         <v>45601</v>
@@ -977,171 +1018,176 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="A1:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="202.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="202.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="202.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" ht="202.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="202.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+      <c r="E5" s="5"/>
+      <c r="F5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:7" ht="202.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B6" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="202.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="202.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" ht="202.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F5" s="5" t="s">
+      <c r="F7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="1:7" ht="202.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>8</v>
+      <c r="C8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>7</v>
@@ -1149,129 +1195,180 @@
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>9</v>
+      <c r="A9" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="E9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="10" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>8</v>
+      <c r="A10" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="5" t="s">
+      <c r="A11" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="5" t="s">
+    </row>
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="5" t="s">
+    </row>
+    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" s="5" t="s">
+    </row>
+    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="5" t="s">
+    </row>
+    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="3"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="3:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="D16" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="13"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="4"/>
       <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="9"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="9"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" tooltip="http://localhost:3000/register" display="http://localhost:3000/register" xr:uid="{B4A6B3C0-C8E0-4862-B992-ECD0B44AF09A}"/>
-    <hyperlink ref="C3" r:id="rId2" display="http://localhost:3000/login" xr:uid="{3C4BED39-581C-406B-9EC4-D095BC215FD1}"/>
-    <hyperlink ref="C7" r:id="rId3" xr:uid="{8979FC6B-EEFF-42A0-86E3-76A765490D2C}"/>
-    <hyperlink ref="C8" r:id="rId4" tooltip="http://localhost:3000/befizetesek/:uazon" display="http://localhost:3000/befizetesek/:uazon" xr:uid="{4BBD2E34-3C21-414F-BD5B-C5CF31968AC0}"/>
-    <hyperlink ref="C9" r:id="rId5" tooltip="http://localhost:3000/befizetes" display="http://localhost:3000/befizetes" xr:uid="{2A10A3F5-2FFA-447B-8949-4C5041458909}"/>
-    <hyperlink ref="C10" r:id="rId6" tooltip="http://localhost:3000/ugyfelek/:uazon" display="http://localhost:3000/ugyfelek/:uazon" xr:uid="{481C7B99-3E34-45C0-87A9-39F40D4A28DB}"/>
-    <hyperlink ref="C11" r:id="rId7" tooltip="http://localhost:3000/tagsagok" display="http://localhost:3000/tagsagok" xr:uid="{42136A81-F8CF-473D-8E9E-21DC13CF4C06}"/>
-    <hyperlink ref="C12" r:id="rId8" tooltip="http://localhost:3000/tagsagok/:uazon" display="http://localhost:3000/tagsagok/:uazon" xr:uid="{553FCC08-36F5-4DB6-8227-D31E52F3AC01}"/>
-    <hyperlink ref="C13" r:id="rId9" tooltip="http://localhost:3000/jelenlet" display="http://localhost:3000/jelenlet" xr:uid="{6F9C0EBC-66BE-4AA9-90D2-2D5D02E34603}"/>
-    <hyperlink ref="C14" r:id="rId10" tooltip="http://localhost:3000/jelenlet" display="http://localhost:3000/jelenlet" xr:uid="{C93C9A32-21C3-4EBA-B94A-AF708F290A08}"/>
-    <hyperlink ref="C15" r:id="rId11" tooltip="http://localhost:3000/jelenlet" display="http://localhost:3000/jelenlet" xr:uid="{EAC0D66C-FBDE-4D16-B16F-CD7DA1B73197}"/>
-    <hyperlink ref="C5" r:id="rId12" xr:uid="{2BB09C3C-6AC9-4E94-9B17-F9F8EE1791FF}"/>
-    <hyperlink ref="C6" r:id="rId13" xr:uid="{211B1958-3A67-4019-9831-AB0511D14F2D}"/>
-    <hyperlink ref="C4" r:id="rId14" xr:uid="{4321C83D-1BDA-4EBA-A27B-CD2466789715}"/>
+    <hyperlink ref="D2" r:id="rId1" tooltip="http://localhost:3000/register" display="http://localhost:3000/register" xr:uid="{B4A6B3C0-C8E0-4862-B992-ECD0B44AF09A}"/>
+    <hyperlink ref="D3" r:id="rId2" display="http://localhost:3000/login" xr:uid="{3C4BED39-581C-406B-9EC4-D095BC215FD1}"/>
+    <hyperlink ref="D7" r:id="rId3" xr:uid="{8979FC6B-EEFF-42A0-86E3-76A765490D2C}"/>
+    <hyperlink ref="D8" r:id="rId4" xr:uid="{4BBD2E34-3C21-414F-BD5B-C5CF31968AC0}"/>
+    <hyperlink ref="D9" r:id="rId5" xr:uid="{2A10A3F5-2FFA-447B-8949-4C5041458909}"/>
+    <hyperlink ref="D10" r:id="rId6" xr:uid="{481C7B99-3E34-45C0-87A9-39F40D4A28DB}"/>
+    <hyperlink ref="D11" r:id="rId7" xr:uid="{42136A81-F8CF-473D-8E9E-21DC13CF4C06}"/>
+    <hyperlink ref="D12" r:id="rId8" xr:uid="{553FCC08-36F5-4DB6-8227-D31E52F3AC01}"/>
+    <hyperlink ref="D13" r:id="rId9" tooltip="http://localhost:3000/jelenlet" display="http://localhost:3000/jelenlet" xr:uid="{6F9C0EBC-66BE-4AA9-90D2-2D5D02E34603}"/>
+    <hyperlink ref="D14" r:id="rId10" xr:uid="{C93C9A32-21C3-4EBA-B94A-AF708F290A08}"/>
+    <hyperlink ref="D5" r:id="rId11" xr:uid="{2BB09C3C-6AC9-4E94-9B17-F9F8EE1791FF}"/>
+    <hyperlink ref="D6" r:id="rId12" xr:uid="{211B1958-3A67-4019-9831-AB0511D14F2D}"/>
+    <hyperlink ref="D4" r:id="rId13" xr:uid="{4321C83D-1BDA-4EBA-A27B-CD2466789715}"/>
+    <hyperlink ref="D15" r:id="rId14" xr:uid="{3EF3EFCF-A79C-4961-B611-3F4C910EFEBC}"/>
+    <hyperlink ref="D16" r:id="rId15" xr:uid="{42A6F1E9-B970-4F2B-811A-E1236C698638}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>